<commit_message>
add some useless function
add some useless function
</commit_message>
<xml_diff>
--- a/doc/系统占用内存分布.xlsx
+++ b/doc/系统占用内存分布.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mayx-my.sharepoint.com/personal/kalinote_say-huahuo_com/Documents/Projects/OSProject/KalinoteOS/KalinoteOS1.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{1332AD0C-3690-4CFE-87A4-E2C4C5921EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FDCF5A1-E2C4-400A-9618-12BCC3752C2A}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{1332AD0C-3690-4CFE-87A4-E2C4C5921EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3050A6B3-C7E6-4518-A399-B9B1C22B2EA3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -282,10 +282,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>注6：这里面还包含一段内存管理表，所在位置是0x003C0000 - 0x003C7FFF (32KB)</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>基本内存
 0x00000 - 0x9FFFF
 (640K)
@@ -346,10 +342,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>JP字体缓存</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>0x10FE8</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -412,10 +404,6 @@
       </rPr>
       <t>[注2]</t>
     </r>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>注2：这一块本来是为IDE硬盘预留的读写缓冲区，但是情况有变，详细使用情况见下表：</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -482,6 +470,19 @@
   </si>
   <si>
     <t>注3：这里是把整个软盘的内容复制到0x100200 - 0x26F7FF这段扩展内存中(虚拟盘)，实际上可能有剩余空间，不会占完</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>注6：这一段内存中从0x3C0000开始有一段内存管理表(32MB内存管理表占用32KB)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>注2：这一块本来是为IDE硬盘预留的读写缓冲区，但是情况有变，详细使用情况见下表(硬盘驱动暂时还没有完成):</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>JP字体缓存
+(可能需要重新找位置)</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -800,6 +801,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -809,6 +819,42 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -818,68 +864,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1179,8 +1180,8 @@
   </sheetPr>
   <dimension ref="A1:V100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:K48"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1193,19 +1194,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="39"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="15"/>
       <c r="L1" s="5"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
@@ -1218,25 +1219,25 @@
       <c r="U1" s="6"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="25" t="s">
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="26"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
@@ -1250,19 +1251,19 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="13" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="28"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="7"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -1275,19 +1276,19 @@
       <c r="U3" s="8"/>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22"/>
       <c r="L4" s="7"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
@@ -1300,19 +1301,19 @@
       <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="13" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="28"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="22"/>
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -1325,19 +1326,19 @@
       <c r="U5" s="8"/>
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="15" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="22"/>
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -1350,19 +1351,19 @@
       <c r="U6" s="8"/>
     </row>
     <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="13" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="28"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="22"/>
       <c r="L7" s="7"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
@@ -1375,19 +1376,19 @@
       <c r="U7" s="8"/>
     </row>
     <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="15" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="28"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="22"/>
       <c r="L8" s="7"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -1400,19 +1401,19 @@
       <c r="U8" s="8"/>
     </row>
     <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="13" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="22"/>
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -1425,19 +1426,19 @@
       <c r="U9" s="8"/>
     </row>
     <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="15" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="28"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="22"/>
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
@@ -1450,19 +1451,19 @@
       <c r="U10" s="8"/>
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="13" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="28"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
       <c r="L11" s="7"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -1478,16 +1479,16 @@
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="28"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
@@ -1500,19 +1501,19 @@
       <c r="U12" s="8"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="28"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
       <c r="L13" s="7"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
@@ -1525,19 +1526,19 @@
       <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="15" t="s">
+      <c r="A14" s="16"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="28"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="22"/>
       <c r="L14" s="7"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -1553,16 +1554,16 @@
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="28"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
       <c r="L15" s="7"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -1578,16 +1579,16 @@
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="22"/>
       <c r="L16" s="7"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
@@ -1603,16 +1604,16 @@
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="28"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="22"/>
       <c r="L17" s="7"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -1628,16 +1629,16 @@
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="28"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
       <c r="L18" s="7"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
@@ -1653,16 +1654,16 @@
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="28"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="22"/>
       <c r="L19" s="7"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
@@ -1678,16 +1679,16 @@
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="28"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="22"/>
       <c r="L20" s="9"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
@@ -1703,18 +1704,18 @@
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="28"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="22"/>
       <c r="L21" s="9"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
@@ -1730,20 +1731,20 @@
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="28"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="9"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
@@ -1756,21 +1757,21 @@
       <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="36"/>
+      <c r="C23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="28"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="22"/>
       <c r="L23" s="9"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
@@ -1783,19 +1784,19 @@
       <c r="U23" s="10"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="13" t="s">
+      <c r="A24" s="16"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="28"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
       <c r="L24" s="9"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
@@ -1808,23 +1809,23 @@
       <c r="U24" s="10"/>
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="28"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="22"/>
       <c r="L25" s="9"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
@@ -1837,19 +1838,19 @@
       <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="13" t="s">
+      <c r="A26" s="16"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="28"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="22"/>
       <c r="L26" s="9"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
@@ -1862,19 +1863,19 @@
       <c r="U26" s="10"/>
     </row>
     <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="13" t="s">
+      <c r="A27" s="16"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="28"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="22"/>
       <c r="L27" s="9"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
@@ -1890,16 +1891,16 @@
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="28"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="22"/>
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
@@ -1915,16 +1916,16 @@
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="28"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="22"/>
       <c r="L29" s="9"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
@@ -1940,18 +1941,18 @@
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="13" t="s">
+      <c r="B30" s="39"/>
+      <c r="C30" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="29"/>
-      <c r="K30" s="30"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="24"/>
       <c r="L30" s="9"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
@@ -1964,11 +1965,11 @@
       <c r="U30" s="10"/>
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>71</v>
+      <c r="B31" s="32" t="s">
+        <v>69</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>36</v>
@@ -1979,10 +1980,10 @@
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
-      <c r="J31" s="31" t="s">
+      <c r="J31" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K31" s="32"/>
+      <c r="K31" s="26"/>
       <c r="L31" s="9"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
@@ -1995,19 +1996,19 @@
       <c r="U31" s="10"/>
     </row>
     <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="18" t="s">
+      <c r="A32" s="16"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="34"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="28"/>
       <c r="L32" s="9"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
@@ -2020,19 +2021,19 @@
       <c r="U32" s="10"/>
     </row>
     <row r="33" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="33"/>
-      <c r="K33" s="34"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="28"/>
       <c r="L33" s="9"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
@@ -2045,19 +2046,19 @@
       <c r="U33" s="10"/>
     </row>
     <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="16"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="13" t="s">
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="33"/>
-      <c r="K34" s="34"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="28"/>
       <c r="L34" s="9"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
@@ -2070,19 +2071,19 @@
       <c r="U34" s="10"/>
     </row>
     <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="16"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="13" t="s">
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="34"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28"/>
       <c r="L35" s="9"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
@@ -2095,19 +2096,19 @@
       <c r="U35" s="10"/>
     </row>
     <row r="36" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="16"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18" t="s">
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="33"/>
-      <c r="K36" s="34"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="28"/>
       <c r="L36" s="9"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
@@ -2123,18 +2124,18 @@
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="13" t="s">
+      <c r="B37" s="32"/>
+      <c r="C37" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="33"/>
-      <c r="K37" s="34"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="28"/>
       <c r="L37" s="9"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
@@ -2147,21 +2148,21 @@
       <c r="U37" s="10"/>
     </row>
     <row r="38" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="34"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="28"/>
       <c r="L38" s="9"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
@@ -2174,17 +2175,17 @@
       <c r="U38" s="10"/>
     </row>
     <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="35"/>
-      <c r="K39" s="36"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="16"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="30"/>
       <c r="L39" s="9"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
@@ -2197,19 +2198,19 @@
       <c r="U39" s="10"/>
     </row>
     <row r="40" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
       <c r="L40" s="7"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -2222,34 +2223,34 @@
       <c r="U40" s="8"/>
     </row>
     <row r="41" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
+      <c r="A41" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
     </row>
     <row r="42" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C42" s="12"/>
       <c r="D42" s="12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G42" s="12"/>
       <c r="H42" s="12"/>
@@ -2259,18 +2260,18 @@
     </row>
     <row r="43" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C43" s="12"/>
       <c r="D43" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E43" s="12"/>
       <c r="F43" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
@@ -2280,7 +2281,7 @@
     </row>
     <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -2295,7 +2296,7 @@
     </row>
     <row r="45" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
@@ -2309,252 +2310,252 @@
       <c r="K45" s="12"/>
     </row>
     <row r="46" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+    </row>
+    <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+    </row>
+    <row r="48" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+    </row>
+    <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+    </row>
+    <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+    </row>
+    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+    </row>
+    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K52" s="16"/>
+    </row>
+    <row r="53" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53" s="16"/>
+      <c r="D53" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" s="16"/>
+      <c r="F53" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-    </row>
-    <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-    </row>
-    <row r="48" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-    </row>
-    <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-    </row>
-    <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-    </row>
-    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-    </row>
-    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+      <c r="G53" s="16"/>
+      <c r="H53" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K53" s="16"/>
+    </row>
+    <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="16"/>
+      <c r="D54" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" s="16"/>
+      <c r="F54" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K54" s="16"/>
+    </row>
+    <row r="55" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E52" s="12"/>
-      <c r="F52" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G52" s="13"/>
-      <c r="H52" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I52" s="12"/>
-      <c r="J52" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="K52" s="12"/>
-    </row>
-    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E53" s="12"/>
-      <c r="F53" s="13" t="s">
+      <c r="B55" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="G53" s="13"/>
-      <c r="H53" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="I53" s="12"/>
-      <c r="J53" s="12" t="s">
+      <c r="C55" s="16"/>
+      <c r="D55" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="K53" s="12"/>
-    </row>
-    <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="E54" s="13"/>
-      <c r="F54" s="12" t="s">
+      <c r="E55" s="16"/>
+      <c r="F55" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="G54" s="12"/>
-      <c r="H54" s="13" t="s">
+      <c r="I55" s="16"/>
+      <c r="J55" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="K54" s="13"/>
-    </row>
-    <row r="55" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B55" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E55" s="13"/>
-      <c r="F55" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="G55" s="12"/>
-      <c r="H55" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="K55" s="13"/>
+      <c r="K55" s="16"/>
     </row>
     <row r="56" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+    </row>
+    <row r="57" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
-      <c r="H56" s="12"/>
-      <c r="I56" s="12"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-    </row>
-    <row r="57" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
-      <c r="H57" s="12"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="16"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
     </row>
     <row r="58" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
-      <c r="K58" s="20"/>
+      <c r="A58" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
     </row>
     <row r="59" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="20"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="20"/>
-      <c r="J59" s="20"/>
-      <c r="K59" s="20"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
     </row>
     <row r="60" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2599,16 +2600,79 @@
     <row r="100" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="99">
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="A47:K47"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="J52:K52"/>
+    <mergeCell ref="J53:K53"/>
+    <mergeCell ref="A46:K46"/>
+    <mergeCell ref="A48:K48"/>
+    <mergeCell ref="A49:K49"/>
+    <mergeCell ref="A50:K50"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="C27:I29"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C14:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A58:K59"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="B2:B21"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="J2:K30"/>
+    <mergeCell ref="J31:K39"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="C38:I39"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="B31:B39"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="C32:I33"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C23:I23"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="J54:K54"/>
     <mergeCell ref="J55:K55"/>
@@ -2625,79 +2689,16 @@
     <mergeCell ref="J44:K44"/>
     <mergeCell ref="F54:G54"/>
     <mergeCell ref="F55:G55"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="J2:K30"/>
-    <mergeCell ref="J31:K39"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C14:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A58:K59"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="B2:B21"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="C38:I39"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="B31:B39"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="C32:I33"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="C27:I29"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="A47:K47"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="A46:K46"/>
-    <mergeCell ref="A48:K48"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A50:K50"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F57:G57"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add Zero Division Exception
add Zero Division Exception
</commit_message>
<xml_diff>
--- a/doc/系统占用内存分布.xlsx
+++ b/doc/系统占用内存分布.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mayx-my.sharepoint.com/personal/kalinote_say-huahuo_com/Documents/Projects/OSProject/KalinoteOS/KalinoteOS1.0/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{1332AD0C-3690-4CFE-87A4-E2C4C5921EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3050A6B3-C7E6-4518-A399-B9B1C22B2EA3}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{1332AD0C-3690-4CFE-87A4-E2C4C5921EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87E4AB69-8602-45EE-9748-C590D965335F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="94">
   <si>
     <t>0x00400 - 0x004FF (256Byte)：BIOS数据区</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -310,10 +310,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>注8：这一块区域在系统进入32位保护模式后，还有部分系统数据储存于此，分别如下：</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>0x00FEC</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -483,6 +479,26 @@
   <si>
     <t>JP字体缓存
 (可能需要重新找位置)</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCI设备信息</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCI设备信息结构体</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x35000</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>注8：这一块区域在系统进入32位保护模式后，还有部分系统数据储存于此(后续可能还需要调整)，分别如下：</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x45000</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -771,7 +787,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -799,7 +815,79 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -810,77 +898,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1181,7 +1203,7 @@
   <dimension ref="A1:V100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+      <selection activeCell="H56" sqref="H56:I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1194,19 +1216,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="15"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="39"/>
       <c r="L1" s="5"/>
       <c r="M1" s="6"/>
       <c r="N1" s="6"/>
@@ -1219,25 +1241,25 @@
       <c r="U1" s="6"/>
     </row>
     <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19" t="s">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="20"/>
+      <c r="K2" s="24"/>
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
@@ -1251,19 +1273,19 @@
       <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="16" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
       <c r="L3" s="7"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -1276,19 +1298,19 @@
       <c r="U3" s="8"/>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="18" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="22"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="26"/>
       <c r="L4" s="7"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
@@ -1301,19 +1323,19 @@
       <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="16" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="22"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
       <c r="L5" s="7"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -1326,19 +1348,19 @@
       <c r="U5" s="8"/>
     </row>
     <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="18" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="22"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
       <c r="L6" s="7"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -1351,19 +1373,19 @@
       <c r="U6" s="8"/>
     </row>
     <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="16" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="22"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="26"/>
       <c r="L7" s="7"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
@@ -1376,19 +1398,19 @@
       <c r="U7" s="8"/>
     </row>
     <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="18" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="22"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="26"/>
       <c r="L8" s="7"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -1401,19 +1423,19 @@
       <c r="U8" s="8"/>
     </row>
     <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="16" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="22"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
       <c r="L9" s="7"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -1426,19 +1448,19 @@
       <c r="U9" s="8"/>
     </row>
     <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="18" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="26"/>
       <c r="L10" s="7"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
@@ -1451,19 +1473,19 @@
       <c r="U10" s="8"/>
     </row>
     <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="16"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="16" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="26"/>
       <c r="L11" s="7"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -1479,16 +1501,16 @@
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="26"/>
       <c r="L12" s="7"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
@@ -1501,19 +1523,19 @@
       <c r="U12" s="8"/>
     </row>
     <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="22"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
       <c r="L13" s="7"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
@@ -1526,19 +1548,19 @@
       <c r="U13" s="8"/>
     </row>
     <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="16"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="18" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="22"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
       <c r="L14" s="7"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
@@ -1554,16 +1576,16 @@
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="26"/>
       <c r="L15" s="7"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -1579,16 +1601,16 @@
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
       <c r="L16" s="7"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
@@ -1604,16 +1626,16 @@
       <c r="A17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="38"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="26"/>
       <c r="L17" s="7"/>
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
@@ -1629,16 +1651,16 @@
       <c r="A18" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="26"/>
       <c r="L18" s="7"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
@@ -1654,16 +1676,16 @@
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
       <c r="L19" s="7"/>
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
@@ -1679,16 +1701,16 @@
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="25"/>
+      <c r="K20" s="26"/>
       <c r="L20" s="9"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
@@ -1704,18 +1726,18 @@
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="22"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26"/>
       <c r="L21" s="9"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
@@ -1731,20 +1753,20 @@
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="22"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="26"/>
       <c r="L22" s="9"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
@@ -1757,21 +1779,21 @@
       <c r="U22" s="10"/>
     </row>
     <row r="23" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="16" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="22"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
       <c r="L23" s="9"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
@@ -1784,19 +1806,19 @@
       <c r="U23" s="10"/>
     </row>
     <row r="24" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="16" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="22"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="26"/>
       <c r="L24" s="9"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
@@ -1809,23 +1831,23 @@
       <c r="U24" s="10"/>
     </row>
     <row r="25" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="39" t="s">
+      <c r="B25" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="22"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="26"/>
       <c r="L25" s="9"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
@@ -1838,19 +1860,19 @@
       <c r="U25" s="10"/>
     </row>
     <row r="26" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="16" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="22"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="25"/>
+      <c r="K26" s="26"/>
       <c r="L26" s="9"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
@@ -1863,19 +1885,19 @@
       <c r="U26" s="10"/>
     </row>
     <row r="27" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="16"/>
-      <c r="B27" s="39"/>
-      <c r="C27" s="16" t="s">
+      <c r="A27" s="12"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="22"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="26"/>
       <c r="L27" s="9"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
@@ -1891,16 +1913,16 @@
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="22"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="26"/>
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
@@ -1916,16 +1938,16 @@
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="22"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="26"/>
       <c r="L29" s="9"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
@@ -1941,18 +1963,18 @@
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="16" t="s">
+      <c r="B30" s="17"/>
+      <c r="C30" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="24"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="28"/>
       <c r="L30" s="9"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
@@ -1965,25 +1987,25 @@
       <c r="U30" s="10"/>
     </row>
     <row r="31" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="12" t="s">
+      <c r="B31" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="25" t="s">
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="K31" s="26"/>
+      <c r="K31" s="30"/>
       <c r="L31" s="9"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
@@ -1996,19 +2018,19 @@
       <c r="U31" s="10"/>
     </row>
     <row r="32" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="33" t="s">
+      <c r="A32" s="12"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="28"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="32"/>
       <c r="L32" s="9"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
@@ -2021,19 +2043,19 @@
       <c r="U32" s="10"/>
     </row>
     <row r="33" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="28"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="32"/>
       <c r="L33" s="9"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
@@ -2046,19 +2068,19 @@
       <c r="U33" s="10"/>
     </row>
     <row r="34" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="31"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="16" t="s">
+      <c r="A34" s="35"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="28"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="32"/>
       <c r="L34" s="9"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
@@ -2071,19 +2093,19 @@
       <c r="U34" s="10"/>
     </row>
     <row r="35" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="31"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="16" t="s">
+      <c r="A35" s="35"/>
+      <c r="B35" s="36"/>
+      <c r="C35" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="28"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="32"/>
       <c r="L35" s="9"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
@@ -2096,19 +2118,19 @@
       <c r="U35" s="10"/>
     </row>
     <row r="36" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="31"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="33" t="s">
+      <c r="A36" s="35"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="33"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="33"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="28"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="32"/>
       <c r="L36" s="9"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
@@ -2124,18 +2146,18 @@
       <c r="A37" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="16" t="s">
+      <c r="B37" s="36"/>
+      <c r="C37" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="28"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="32"/>
       <c r="L37" s="9"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
@@ -2148,21 +2170,21 @@
       <c r="U37" s="10"/>
     </row>
     <row r="38" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="32"/>
-      <c r="C38" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="28"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="31"/>
+      <c r="K38" s="32"/>
       <c r="L38" s="9"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
@@ -2175,17 +2197,17 @@
       <c r="U38" s="10"/>
     </row>
     <row r="39" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="31"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="30"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="34"/>
       <c r="L39" s="9"/>
       <c r="M39" s="10"/>
       <c r="N39" s="10"/>
@@ -2198,19 +2220,19 @@
       <c r="U39" s="10"/>
     </row>
     <row r="40" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
-      <c r="J40" s="17"/>
-      <c r="K40" s="17"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14"/>
       <c r="L40" s="7"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -2223,339 +2245,347 @@
       <c r="U40" s="8"/>
     </row>
     <row r="41" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="17"/>
+      <c r="A41" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
     </row>
     <row r="42" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12" t="s">
+      <c r="E42" s="13"/>
+      <c r="F42" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
     </row>
     <row r="43" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
-      <c r="K43" s="12"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
     </row>
     <row r="44" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
-      <c r="K44" s="12"/>
+        <v>55</v>
+      </c>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
     </row>
     <row r="45" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
+        <v>56</v>
+      </c>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
     </row>
     <row r="46" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+      <c r="K46" s="14"/>
+    </row>
+    <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+    </row>
+    <row r="48" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+      <c r="K48" s="14"/>
+    </row>
+    <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="17"/>
-    </row>
-    <row r="47" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-    </row>
-    <row r="48" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
-      <c r="J48" s="17"/>
-      <c r="K48" s="17"/>
-    </row>
-    <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="17"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
-      <c r="J49" s="17"/>
-      <c r="K49" s="17"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
     </row>
     <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
-      <c r="J50" s="17"/>
-      <c r="K50" s="17"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+      <c r="K50" s="14"/>
     </row>
     <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
-      <c r="J51" s="17"/>
-      <c r="K51" s="17"/>
+      <c r="A51" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
     </row>
     <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="I52" s="16"/>
-      <c r="J52" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K52" s="16"/>
+      <c r="B52" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="12"/>
+      <c r="D52" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K52" s="12"/>
     </row>
     <row r="53" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B53" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E53" s="16"/>
-      <c r="F53" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I53" s="16"/>
-      <c r="J53" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="K53" s="16"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K53" s="12"/>
     </row>
     <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E54" s="16"/>
-      <c r="F54" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="I54" s="16"/>
-      <c r="J54" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K54" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="B54" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="K54" s="12"/>
     </row>
     <row r="55" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B55" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E55" s="16"/>
-      <c r="F55" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G55" s="16"/>
-      <c r="H55" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="I55" s="16"/>
-      <c r="J55" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="K55" s="16"/>
+        <v>56</v>
+      </c>
+      <c r="B55" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="K55" s="12"/>
     </row>
     <row r="56" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="16"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="16"/>
-      <c r="K56" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="41"/>
+      <c r="D56" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
     </row>
     <row r="57" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="16"/>
-      <c r="K57" s="16"/>
+        <v>56</v>
+      </c>
+      <c r="B57" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="41"/>
+      <c r="D57" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
     </row>
     <row r="58" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="37"/>
-      <c r="C58" s="37"/>
-      <c r="D58" s="37"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="37"/>
+      <c r="A58" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="21"/>
     </row>
     <row r="59" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="37"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
-      <c r="K59" s="37"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
     </row>
     <row r="60" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2600,6 +2630,89 @@
     <row r="100" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="99">
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="J55:K55"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C11:I13"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="C38:I39"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="B31:B39"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="C32:I33"/>
+    <mergeCell ref="A58:K59"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="B2:B21"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="J2:K30"/>
+    <mergeCell ref="J31:K39"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C10:I10"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="C27:I29"/>
+    <mergeCell ref="B25:B30"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C14:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="D54:E54"/>
@@ -2616,89 +2729,6 @@
     <mergeCell ref="D52:E52"/>
     <mergeCell ref="F52:G52"/>
     <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="C10:I10"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="C27:I29"/>
-    <mergeCell ref="B25:B30"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C14:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A58:K59"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="B2:B21"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C8:I8"/>
-    <mergeCell ref="J2:K30"/>
-    <mergeCell ref="J31:K39"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="C38:I39"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="B31:B39"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="C32:I33"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="C11:I13"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F57:G57"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>